<commit_message>
Add relationship between entites, fix a minor error with excel2json algorithm
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Déjà dans l'emploi" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Déjà dans l''emploi'!$A$1:$Z$3</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Déjà dans l''emploi'!$A$1:$Y$3</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="52">
   <si>
     <t xml:space="preserve">Matricule</t>
   </si>
@@ -100,9 +100,6 @@
     <t xml:space="preserve">PRENOM N2</t>
   </si>
   <si>
-    <t xml:space="preserve">Type Assessment</t>
-  </si>
-  <si>
     <t xml:space="preserve">FARFAOUA</t>
   </si>
   <si>
@@ -118,9 +115,6 @@
     <t xml:space="preserve">SUPPORT ADMINISTRATIF</t>
   </si>
   <si>
-    <t xml:space="preserve">&gt;5</t>
-  </si>
-  <si>
     <t xml:space="preserve">xoxox</t>
   </si>
   <si>
@@ -167,16 +161,36 @@
   </si>
   <si>
     <t xml:space="preserve">GHANAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ILHAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHAHIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DRISS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOUSOUFA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MESSI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIONEL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
-    <numFmt numFmtId="166" formatCode="0"/>
+    <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
+    <numFmt numFmtId="166" formatCode="[$-40C]dd/mm/yyyy"/>
+    <numFmt numFmtId="167" formatCode="m/d/yyyy"/>
+    <numFmt numFmtId="168" formatCode="0"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -184,7 +198,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -206,7 +219,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri Light"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -214,24 +226,21 @@
       <color rgb="FF000000"/>
       <name val="Calibri Light"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Calibri Light"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri Light"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -253,7 +262,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA9D18E"/>
-        <bgColor rgb="FFC5E0B4"/>
+        <bgColor rgb="FF99CCFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -262,14 +271,8 @@
         <bgColor rgb="FFF4B183"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC5E0B4"/>
-        <bgColor rgb="FFA9D18E"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="8">
+  <borders count="6">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -287,13 +290,6 @@
     <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
       <right style="thin"/>
-      <top style="medium"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="medium"/>
       <top style="medium"/>
       <bottom style="thin"/>
       <diagonal/>
@@ -319,13 +315,6 @@
       <bottom style="thin"/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="medium"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -352,7 +341,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -365,6 +354,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -373,11 +366,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -385,59 +378,59 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -490,7 +483,7 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFC5E0B4"/>
+      <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFF4B183"/>
@@ -526,392 +519,642 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z12"/>
+  <dimension ref="A1:AMJ12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="U1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Z9" activeCellId="0" sqref="Z9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="1" style="1" width="11.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="27.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="25.81"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="11.45"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="11.45"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="35.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.72"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="11.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="19.18"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="25" min="13" style="1" width="11.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="37.82"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="1" width="11.45"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="13" style="1" width="11.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" s="7" customFormat="true" ht="64.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+    <row r="1" s="8" customFormat="true" ht="64.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="U1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="V1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="W1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="X1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Y1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" s="20" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="n">
+      <c r="A2" s="9" t="n">
         <v>1111111</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="D2" s="11" t="n">
+        <v>27941</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="10" t="n">
-        <v>27941</v>
-      </c>
-      <c r="E2" s="10" t="s">
+      <c r="F2" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="G2" s="12" t="n">
+        <v>39661</v>
+      </c>
+      <c r="H2" s="10" t="n">
+        <v>300</v>
+      </c>
+      <c r="I2" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="11" t="n">
-        <v>39661</v>
-      </c>
-      <c r="H2" s="9" t="n">
-        <v>300</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="J2" s="13" t="n">
+      <c r="J2" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="K2" s="14" t="n">
+      <c r="K2" s="15" t="n">
         <v>44624</v>
       </c>
-      <c r="L2" s="15" t="n">
+      <c r="L2" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="M2" s="14" t="n">
+      <c r="M2" s="15" t="n">
         <v>44562</v>
       </c>
-      <c r="N2" s="16" t="n">
+      <c r="N2" s="17" t="n">
         <v>100</v>
       </c>
-      <c r="O2" s="16" t="n">
+      <c r="O2" s="17" t="n">
         <v>100</v>
       </c>
-      <c r="P2" s="16" t="n">
+      <c r="P2" s="17" t="n">
         <v>100</v>
       </c>
-      <c r="Q2" s="17" t="n">
+      <c r="Q2" s="18" t="n">
         <f aca="false">(N2+O2+P2)/3</f>
         <v>100</v>
       </c>
-      <c r="R2" s="13" t="n">
+      <c r="R2" s="14" t="n">
         <v>4</v>
       </c>
-      <c r="S2" s="15" t="s">
+      <c r="S2" s="16" t="n">
+        <v>8</v>
+      </c>
+      <c r="T2" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="U2" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="T2" s="18" t="s">
+      <c r="V2" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="U2" s="9" t="s">
+      <c r="W2" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="V2" s="9" t="s">
+      <c r="X2" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="W2" s="9" t="s">
+      <c r="Y2" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="X2" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y2" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="Z2" s="19"/>
+      <c r="AMJ2" s="0"/>
     </row>
     <row r="3" s="20" customFormat="true" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="n">
+      <c r="A3" s="9" t="n">
         <v>2222222</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="11" t="n">
+        <v>27085</v>
+      </c>
+      <c r="E3" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="F3" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="12" t="n">
+        <v>39937</v>
+      </c>
+      <c r="H3" s="10" t="n">
+        <v>567</v>
+      </c>
+      <c r="I3" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="10" t="n">
-        <v>27085</v>
-      </c>
-      <c r="E3" s="10" t="s">
+      <c r="J3" s="14" t="n">
+        <v>5</v>
+      </c>
+      <c r="K3" s="15" t="n">
+        <v>44625</v>
+      </c>
+      <c r="L3" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="M3" s="15" t="n">
+        <v>43893</v>
+      </c>
+      <c r="N3" s="17" t="n">
+        <v>89</v>
+      </c>
+      <c r="O3" s="17" t="n">
+        <v>90</v>
+      </c>
+      <c r="P3" s="17" t="n">
+        <v>100</v>
+      </c>
+      <c r="Q3" s="18" t="n">
+        <f aca="false">(N3+O3+P3)/3</f>
+        <v>93</v>
+      </c>
+      <c r="R3" s="14" t="n">
+        <v>5</v>
+      </c>
+      <c r="S3" s="14" t="n">
+        <v>3</v>
+      </c>
+      <c r="T3" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" s="11" t="n">
-        <v>39937</v>
-      </c>
-      <c r="H3" s="9" t="n">
-        <v>567</v>
-      </c>
-      <c r="I3" s="12" t="s">
+      <c r="U3" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="V3" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="J3" s="13" t="n">
-        <v>5</v>
-      </c>
-      <c r="K3" s="14" t="n">
-        <v>44625</v>
-      </c>
-      <c r="L3" s="15" t="n">
-        <v>2</v>
-      </c>
-      <c r="M3" s="14" t="n">
-        <v>43893</v>
-      </c>
-      <c r="N3" s="16" t="n">
-        <v>100</v>
-      </c>
-      <c r="O3" s="16" t="n">
-        <v>100</v>
-      </c>
-      <c r="P3" s="16" t="n">
-        <v>100</v>
-      </c>
-      <c r="Q3" s="17" t="n">
-        <f aca="false">(N3+O3+P3)/3</f>
-        <v>100</v>
-      </c>
-      <c r="R3" s="13" t="n">
-        <v>3</v>
-      </c>
-      <c r="S3" s="13" t="n">
-        <v>3</v>
-      </c>
-      <c r="T3" s="18" t="s">
+      <c r="W3" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="U3" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="V3" s="9" t="s">
+      <c r="X3" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="W3" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="X3" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y3" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="Z3" s="19"/>
+      <c r="Y3" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="AMJ3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="21" t="n">
         <v>2226272</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D4" s="21" t="n">
         <v>262626</v>
       </c>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="22"/>
+      <c r="E4" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="12" t="n">
+        <v>39938</v>
+      </c>
+      <c r="H4" s="10" t="n">
+        <v>293</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" s="15" t="n">
+        <v>44626</v>
+      </c>
+      <c r="L4" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="M4" s="15" t="n">
+        <v>43894</v>
+      </c>
+      <c r="N4" s="17" t="n">
+        <v>100</v>
+      </c>
+      <c r="O4" s="17" t="n">
+        <v>80</v>
+      </c>
+      <c r="P4" s="17" t="n">
+        <v>90</v>
+      </c>
+      <c r="Q4" s="18" t="n">
+        <f aca="false">(N4+O4+P4)/3</f>
+        <v>90</v>
+      </c>
+      <c r="R4" s="14" t="n">
+        <v>4</v>
+      </c>
+      <c r="S4" s="14" t="n">
+        <v>4</v>
+      </c>
+      <c r="T4" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="U4" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="V4" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="W4" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="X4" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y4" s="10" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="21"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="22"/>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="21" t="n">
+        <v>3226273</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="21" t="n">
+        <v>112233</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="12" t="n">
+        <v>39939</v>
+      </c>
+      <c r="H5" s="10" t="n">
+        <v>196</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="14" t="n">
+        <v>4</v>
+      </c>
+      <c r="K5" s="15" t="n">
+        <v>44627</v>
+      </c>
+      <c r="L5" s="16" t="n">
+        <v>5</v>
+      </c>
+      <c r="M5" s="15" t="n">
+        <v>43895</v>
+      </c>
+      <c r="N5" s="17" t="n">
+        <v>99</v>
+      </c>
+      <c r="O5" s="17" t="n">
+        <v>88</v>
+      </c>
+      <c r="P5" s="17" t="n">
+        <v>95</v>
+      </c>
+      <c r="Q5" s="18" t="n">
+        <f aca="false">(N5+O5+P5)/3</f>
+        <v>94</v>
+      </c>
+      <c r="R5" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="S5" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="T5" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="U5" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="V5" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="W5" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="X5" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y5" s="10" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="21"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="22"/>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="21" t="n">
+        <v>2276274</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="21" t="n">
+        <v>445566</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="12" t="n">
+        <v>39940</v>
+      </c>
+      <c r="H6" s="10" t="n">
+        <v>222</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6" s="14" t="n">
+        <v>2</v>
+      </c>
+      <c r="K6" s="15" t="n">
+        <v>44628</v>
+      </c>
+      <c r="L6" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="M6" s="15" t="n">
+        <v>43896</v>
+      </c>
+      <c r="N6" s="17" t="n">
+        <v>93</v>
+      </c>
+      <c r="O6" s="17" t="n">
+        <v>79</v>
+      </c>
+      <c r="P6" s="17" t="n">
+        <v>100</v>
+      </c>
+      <c r="Q6" s="18" t="n">
+        <f aca="false">(N6+O6+P6)/3</f>
+        <v>90.6666666666667</v>
+      </c>
+      <c r="R6" s="14" t="n">
+        <v>3</v>
+      </c>
+      <c r="S6" s="14" t="n">
+        <v>2</v>
+      </c>
+      <c r="T6" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="U6" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="V6" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="W6" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="X6" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y6" s="10" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="21"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="22"/>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="21" t="n">
+        <v>4426211</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="21" t="n">
+        <v>778899</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="12" t="n">
+        <v>39941</v>
+      </c>
+      <c r="H7" s="10" t="n">
+        <v>97</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="J7" s="14" t="n">
+        <v>8</v>
+      </c>
+      <c r="K7" s="15" t="n">
+        <v>44629</v>
+      </c>
+      <c r="L7" s="16" t="n">
+        <v>6</v>
+      </c>
+      <c r="M7" s="15" t="n">
+        <v>43897</v>
+      </c>
+      <c r="N7" s="17" t="n">
+        <v>78</v>
+      </c>
+      <c r="O7" s="17" t="n">
+        <v>95</v>
+      </c>
+      <c r="P7" s="17" t="n">
+        <v>90</v>
+      </c>
+      <c r="Q7" s="18" t="n">
+        <f aca="false">(N7+O7+P7)/3</f>
+        <v>87.6666666666667</v>
+      </c>
+      <c r="R7" s="14" t="n">
+        <v>5</v>
+      </c>
+      <c r="S7" s="14" t="n">
+        <v>3</v>
+      </c>
+      <c r="T7" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="U7" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="V7" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="W7" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="X7" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y7" s="10" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="21"/>
       <c r="B8" s="21"/>
       <c r="C8" s="21"/>
       <c r="D8" s="21"/>
       <c r="E8" s="21"/>
       <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
+      <c r="G8" s="22"/>
       <c r="H8" s="21"/>
       <c r="I8" s="21"/>
       <c r="J8" s="21"/>
-      <c r="K8" s="22"/>
+      <c r="K8" s="23"/>
     </row>
-    <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="21"/>
       <c r="B9" s="21"/>
       <c r="C9" s="21"/>
       <c r="D9" s="21"/>
       <c r="E9" s="21"/>
       <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
+      <c r="G9" s="22"/>
       <c r="H9" s="21"/>
       <c r="I9" s="21"/>
       <c r="J9" s="21"/>
-      <c r="K9" s="22"/>
+      <c r="K9" s="23"/>
     </row>
-    <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="21"/>
       <c r="B10" s="21"/>
       <c r="C10" s="21"/>
       <c r="D10" s="21"/>
       <c r="E10" s="21"/>
       <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
+      <c r="G10" s="22"/>
       <c r="H10" s="21"/>
       <c r="I10" s="21"/>
       <c r="J10" s="21"/>
-      <c r="K10" s="22"/>
+      <c r="K10" s="23"/>
     </row>
-    <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="21"/>
       <c r="B11" s="21"/>
       <c r="C11" s="21"/>
       <c r="D11" s="21"/>
       <c r="E11" s="21"/>
       <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
+      <c r="G11" s="22"/>
       <c r="H11" s="21"/>
       <c r="I11" s="21"/>
       <c r="J11" s="21"/>
-      <c r="K11" s="22"/>
+      <c r="K11" s="23"/>
     </row>
-    <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="21"/>
       <c r="B12" s="21"/>
       <c r="C12" s="21"/>
       <c r="D12" s="21"/>
       <c r="E12" s="21"/>
       <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
+      <c r="G12" s="22"/>
       <c r="H12" s="21"/>
       <c r="I12" s="21"/>
       <c r="J12" s="21"/>
-      <c r="K12" s="22"/>
+      <c r="K12" s="23"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Z3"/>
+  <autoFilter ref="A1:Y3"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>